<commit_message>
add date layout for 02/01/2006
</commit_message>
<xml_diff>
--- a/eksel/testdata/data-time.xlsx
+++ b/eksel/testdata/data-time.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Time Start</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/06/1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/06/1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/06/1997</t>
   </si>
 </sst>
 </file>
@@ -45,6 +54,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,16 +114,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,111 +148,125 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.25"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0.509027777777778</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>0.523611111111111</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>35593</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>0.523611111111111</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>0.538194444444444</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>35594</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>0.538194444444444</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.552777777777778</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>35595</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>0.552777777777778</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>0.567361111111111</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>35596</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>0.567361111111111</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>0.581944444444445</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>35597</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>0.581944444444444</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>0.596527777777778</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>35598</v>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>0.596527777777778</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>0.611111111111111</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>35599</v>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>0.611111111111111</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>0.625694444444444</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>35600</v>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>1.61111111111111</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>1.62569444444444</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>50575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>